<commit_message>
GANTT et Top Projet
</commit_message>
<xml_diff>
--- a/AA_Management/00_GANTT/GANTT_V2.xlsx
+++ b/AA_Management/00_GANTT/GANTT_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Documents\STUF-2020\AA_Management\00_GANTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD327D1-D48B-4660-9D63-57FB6D1BD48A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5032EB84-97E2-4909-AAEF-9B2E6AAA0131}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="6" xr2:uid="{B5F72930-40F3-4E46-BBD8-9CE832AB9E95}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{B5F72930-40F3-4E46-BBD8-9CE832AB9E95}"/>
   </bookViews>
   <sheets>
     <sheet name="Recap" sheetId="6" r:id="rId1"/>
@@ -2030,8 +2030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADF6AF9-7A4E-44DD-AE57-99FC9DDD9D66}">
   <dimension ref="A1:AC40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2266,10 +2266,10 @@
       </c>
       <c r="E8">
         <f t="shared" ref="E8:E20" si="0">MAX(F8:AF8)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
@@ -2284,10 +2284,10 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I9">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
@@ -2302,10 +2302,10 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I10">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.3">
@@ -2558,10 +2558,10 @@
       </c>
       <c r="E25">
         <f>MAX(F25:Y25)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
@@ -2606,10 +2606,10 @@
       </c>
       <c r="E28">
         <f>MAX(F28:Y28)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
@@ -2833,7 +2833,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3061,13 +3061,16 @@
       </c>
       <c r="D14">
         <f>MAX(E14:AA14)</f>
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="L14">
         <v>10</v>
       </c>
       <c r="M14">
-        <v>10</v>
+        <v>50</v>
+      </c>
+      <c r="N14">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -3115,13 +3118,19 @@
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="M17">
+        <v>50</v>
+      </c>
+      <c r="N17">
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -3139,6 +3148,12 @@
         <v>50</v>
       </c>
       <c r="L18">
+        <v>50</v>
+      </c>
+      <c r="M18">
+        <v>50</v>
+      </c>
+      <c r="N18">
         <v>50</v>
       </c>
     </row>
@@ -3387,7 +3402,7 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D2:D3 D7:P26 D41:P54 D28:P38 O27:P27">
+  <conditionalFormatting sqref="D2:D3 D41:P54 D28:P38 O27:P27 D7:P26">
     <cfRule type="colorScale" priority="280">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3433,7 +3448,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3570,7 +3585,7 @@
       </c>
       <c r="D7">
         <f t="shared" ref="D7" si="0">MAX(E7:AA7)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="I7">
         <v>20</v>
@@ -3585,10 +3600,10 @@
         <v>40</v>
       </c>
       <c r="M7">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="N7">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -4370,7 +4385,7 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11">
-        <f t="shared" ref="D11:D19" si="0">MAX(E11:AV11)</f>
+        <f t="shared" ref="D11:D15" si="0">MAX(E11:AV11)</f>
         <v>0</v>
       </c>
       <c r="E11" s="2"/>
@@ -4827,8 +4842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{163A8FDE-E8ED-4ACD-9152-9240B748B333}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4844,7 +4859,7 @@
     <col min="9" max="9" width="3.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="3.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.77734375" customWidth="1"/>
@@ -4876,13 +4891,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="34">
-        <v>43531</v>
+        <v>43544</v>
       </c>
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
       <c r="I2" s="33">
         <f>WEEKNUM(F2)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J2" s="33"/>
       <c r="O2" s="2"/>
@@ -5148,6 +5163,12 @@
       <c r="L18">
         <v>0</v>
       </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
@@ -5158,7 +5179,7 @@
       </c>
       <c r="D19">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H19">
         <v>50</v>
@@ -5170,10 +5191,10 @@
         <v>50</v>
       </c>
       <c r="K19">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="L19">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -5197,8 +5218,12 @@
       <c r="L20" s="25">
         <v>50</v>
       </c>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
+      <c r="M20" s="25">
+        <v>50</v>
+      </c>
+      <c r="N20" s="25">
+        <v>50</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
@@ -5237,8 +5262,12 @@
       <c r="L22" s="25">
         <v>30</v>
       </c>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
+      <c r="M22" s="25">
+        <v>30</v>
+      </c>
+      <c r="N22" s="25">
+        <v>30</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
@@ -5262,8 +5291,12 @@
       <c r="L23" s="25">
         <v>20</v>
       </c>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
+      <c r="M23" s="25">
+        <v>20</v>
+      </c>
+      <c r="N23" s="25">
+        <v>20</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>

</xml_diff>